<commit_message>
addition of adhesive properties and some adhesive family properties
</commit_message>
<xml_diff>
--- a/LOT_documents/FAIR Ontology Entities.xlsx
+++ b/LOT_documents/FAIR Ontology Entities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ioannisdasoulas/Desktop/FAIR/Adhesive Selector/adhesive_ontology/LOT_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3F703F-CFD1-7945-8951-4DC66DAAF9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBF9CD4-1106-6B4B-97B1-31707B03EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="960" windowWidth="28020" windowHeight="16060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2600" yWindow="-17680" windowWidth="36480" windowHeight="17140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="394">
   <si>
     <t>Description</t>
   </si>
@@ -415,12 +415,6 @@
     <t>(-80, 80)</t>
   </si>
   <si>
-    <t xml:space="preserve">pot life </t>
-  </si>
-  <si>
-    <t>A relation between an adhesive and the period of time during which it maintains its workable properties after it's been mixed</t>
-  </si>
-  <si>
     <t>minutes</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
     <t>A relation between an adhesive and the maximum thickness it should be applied</t>
   </si>
   <si>
-    <t>open time</t>
-  </si>
-  <si>
     <t>A relation between an adhesive and amount of time after its application to the substrate during which it retains its ability to adhere to and bond</t>
   </si>
   <si>
@@ -526,9 +517,6 @@
     <t>e-modulus</t>
   </si>
   <si>
-    <t>A relation between an adhesive and its material's elasticiry</t>
-  </si>
-  <si>
     <t>MPa</t>
   </si>
   <si>
@@ -580,9 +568,6 @@
     <t>More explanations needed. I would not include for now</t>
   </si>
   <si>
-    <t>minimum temperature resistance</t>
-  </si>
-  <si>
     <t>A relation between an adhesive and the minimum temperature it can withstand</t>
   </si>
   <si>
@@ -592,9 +577,6 @@
     <t>Included as A_Lowest_Allowed_Perf_T</t>
   </si>
   <si>
-    <t>maximum temperature resistance</t>
-  </si>
-  <si>
     <t>A relation between an adhesive and the maximum temperature it can withstand</t>
   </si>
   <si>
@@ -655,9 +637,6 @@
     <t>Included as F_Water_Resistance</t>
   </si>
   <si>
-    <t>Awaiting for definition. IDP KB values not exactly match with data</t>
-  </si>
-  <si>
     <t>uv resistance</t>
   </si>
   <si>
@@ -727,22 +706,7 @@
     <t>maximum application RH</t>
   </si>
   <si>
-    <t xml:space="preserve">minimum curing time </t>
-  </si>
-  <si>
-    <t>A relation between an adhesive type and the minimum amount of time it needs to be cured</t>
-  </si>
-  <si>
     <t>Included as F_Lowest_Allowed_Curing_T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maximum curing time </t>
-  </si>
-  <si>
-    <t>curing hardening time</t>
-  </si>
-  <si>
-    <t>adhesion ferro-metals</t>
   </si>
   <si>
     <t>Defined as part of F_Adhesion</t>
@@ -1162,6 +1126,108 @@
   </si>
   <si>
     <t>A relation between an adhesive and the estimation of its cost per mililiter (ml) based on amount paid for small scale tubes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum pot life </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximum pot life </t>
+  </si>
+  <si>
+    <t>A relation between an adhesive and the maximum period of time during which it maintains its workable properties after it's been mixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A relation between an adhesive and the minimum period of time during which it maintains its workable properties after it's been mixed </t>
+  </si>
+  <si>
+    <t>max open time</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive and its material's elasticity</t>
+  </si>
+  <si>
+    <t>minimum resistance temperature</t>
+  </si>
+  <si>
+    <t>maximum resistance temperature</t>
+  </si>
+  <si>
+    <t>minimum polymer transition temperature</t>
+  </si>
+  <si>
+    <t>maximum polymer transition temperature</t>
+  </si>
+  <si>
+    <t>Minimum estimated temperature at which amorphous polymers undergo a transition from glassy to rubbery state</t>
+  </si>
+  <si>
+    <t>Maximum estimated temperature at which amorphous polymers undergo a transition from glassy to rubbery state</t>
+  </si>
+  <si>
+    <t>minimum shear strength</t>
+  </si>
+  <si>
+    <t>maximum shear strength</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the degree of its shear strength, classified as low, medium or high</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its maximum estimated shear strength</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its minimum estimated shear strength</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its polymer type</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its relative ability to withstand humidity</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its relative ability to withstand water</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its relative ability to withstand chemicals</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its relative ability to withstand shock</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its relative ability to withstand creep</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its minimum relative humidity percentage</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and its maximum relative humidity percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum curing temperature </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximum curing temperature </t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the minimum temperature it can be cured</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the maximum temperature it can be cured</t>
+  </si>
+  <si>
+    <t>Data needs cleaning before integration to KG</t>
+  </si>
+  <si>
+    <t>Included as F_Highest_Allowed_Curing_T</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive family and an estimation of time it requires to cure/harden</t>
+  </si>
+  <si>
+    <t>curing time estimation</t>
+  </si>
+  <si>
+    <t>adhesion quality</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1588,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1546,13 +1612,13 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.15">
@@ -1645,10 +1711,10 @@
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>9</v>
@@ -1656,10 +1722,10 @@
     </row>
     <row r="11" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>8</v>
@@ -1938,10 +2004,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O1004"/>
+  <dimension ref="A1:O1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A64" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1981,13 +2047,13 @@
         <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.15">
@@ -2044,13 +2110,13 @@
     </row>
     <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>17</v>
@@ -2062,7 +2128,7 @@
         <v>60</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -2073,10 +2139,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>66</v>
@@ -2131,7 +2197,7 @@
         <v>73</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>74</v>
@@ -2157,7 +2223,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>74</v>
@@ -2183,7 +2249,7 @@
         <v>109</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>74</v>
@@ -2417,7 +2483,7 @@
         <v>100</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>101</v>
@@ -2443,7 +2509,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>101</v>
@@ -2469,7 +2535,7 @@
         <v>113</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>101</v>
@@ -2495,7 +2561,7 @@
         <v>105</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>101</v>
@@ -2521,7 +2587,7 @@
         <v>107</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>101</v>
@@ -2547,7 +2613,7 @@
         <v>115</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>101</v>
@@ -2573,7 +2639,7 @@
         <v>117</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>101</v>
@@ -2599,7 +2665,7 @@
         <v>119</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>101</v>
@@ -2625,7 +2691,7 @@
         <v>121</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>101</v>
@@ -2671,71 +2737,71 @@
         <v>18</v>
       </c>
       <c r="B28" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A29" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>130</v>
+        <v>361</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>131</v>
+        <v>362</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>62</v>
@@ -2749,19 +2815,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>62</v>
@@ -2770,24 +2836,24 @@
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>62</v>
@@ -2798,255 +2864,248 @@
     </row>
     <row r="33" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A33" s="15" t="s">
-        <v>225</v>
+        <v>18</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>140</v>
+        <v>364</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>226</v>
+        <v>136</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>224</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
     <row r="34" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A34" s="15" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>74</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="1:15" ht="70" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A35" s="15" t="s">
-        <v>18</v>
+        <v>218</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>146</v>
+        <v>220</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>176</v>
+        <v>217</v>
       </c>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="1:15" ht="84" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" ht="70" x14ac:dyDescent="0.15">
       <c r="A36" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>128</v>
+        <v>66</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="1:15" ht="70" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" ht="84" x14ac:dyDescent="0.15">
       <c r="A37" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" ht="70" x14ac:dyDescent="0.15">
       <c r="A38" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>274</v>
+        <v>152</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
     </row>
-    <row r="39" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A39" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>199</v>
+        <v>262</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="H39" s="14"/>
+        <v>154</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>173</v>
+      </c>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
     </row>
-    <row r="40" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A40" s="15" t="s">
-        <v>68</v>
+        <v>218</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>167</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
     </row>
     <row r="41" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>166</v>
+        <v>365</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -3056,30 +3115,30 @@
       <c r="N41" s="14"/>
       <c r="O41" s="14"/>
     </row>
-    <row r="42" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="15" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -3089,30 +3148,30 @@
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
     </row>
-    <row r="43" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -3122,30 +3181,30 @@
       <c r="N43" s="14"/>
       <c r="O43" s="14"/>
     </row>
-    <row r="44" spans="1:15" ht="42" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -3160,24 +3219,26 @@
         <v>18</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="14" t="s">
-        <v>74</v>
+      <c r="E45" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="H45" s="14"/>
+        <v>150</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>176</v>
+      </c>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
       <c r="K45" s="14"/>
@@ -3191,10 +3252,10 @@
         <v>18</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>185</v>
+        <v>366</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>59</v>
@@ -3203,11 +3264,12 @@
         <v>74</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>187</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
       <c r="K46" s="14"/>
@@ -3216,30 +3278,27 @@
       <c r="N46" s="14"/>
       <c r="O46" s="14"/>
     </row>
-    <row r="47" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A47" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>188</v>
+        <v>367</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>189</v>
+        <v>59</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -3249,30 +3308,30 @@
       <c r="N47" s="14"/>
       <c r="O47" s="14"/>
     </row>
-    <row r="48" spans="1:15" ht="84" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A48" s="15" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="G48" s="15" t="s">
         <v>62</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>269</v>
+        <v>166</v>
       </c>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
@@ -3282,31 +3341,29 @@
       <c r="N48" s="14"/>
       <c r="O48" s="14"/>
     </row>
-    <row r="49" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>194</v>
+        <v>368</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>195</v>
+        <v>370</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>196</v>
+        <v>66</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F49" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>198</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H49" s="15"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
@@ -3315,31 +3372,29 @@
       <c r="N49" s="14"/>
       <c r="O49" s="14"/>
     </row>
-    <row r="50" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A50" s="15" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>200</v>
+        <v>369</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>195</v>
+        <v>371</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>159</v>
+      <c r="E50" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>195</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H50" s="15"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
@@ -3348,30 +3403,30 @@
       <c r="N50" s="14"/>
       <c r="O50" s="14"/>
     </row>
-    <row r="51" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:15" ht="84" x14ac:dyDescent="0.15">
       <c r="A51" s="15" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>203</v>
+        <v>62</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>195</v>
+        <v>257</v>
       </c>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
@@ -3381,15 +3436,15 @@
       <c r="N51" s="14"/>
       <c r="O51" s="14"/>
     </row>
-    <row r="52" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A52" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>195</v>
+        <v>374</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>17</v>
@@ -3401,11 +3456,9 @@
         <v>60</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>206</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H52" s="15"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
@@ -3416,29 +3469,27 @@
     </row>
     <row r="53" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A53" s="15" t="s">
-        <v>363</v>
+        <v>19</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>207</v>
+        <v>372</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>365</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H53" s="15"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
@@ -3447,30 +3498,30 @@
       <c r="N53" s="14"/>
       <c r="O53" s="14"/>
     </row>
-    <row r="54" spans="1:15" ht="42" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A54" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>209</v>
+        <v>373</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>195</v>
+        <v>375</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>190</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -3480,31 +3531,29 @@
       <c r="N54" s="14"/>
       <c r="O54" s="14"/>
     </row>
-    <row r="55" spans="1:15" ht="42" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A55" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C55" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="G55" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="D55" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>195</v>
-      </c>
+      <c r="H55" s="15"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
@@ -3518,10 +3567,10 @@
         <v>19</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>195</v>
+        <v>377</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>17</v>
@@ -3529,15 +3578,13 @@
       <c r="E56" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>215</v>
+      <c r="F56" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>195</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="H56" s="15"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
       <c r="K56" s="14"/>
@@ -3551,10 +3598,10 @@
         <v>19</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>195</v>
+        <v>379</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>17</v>
@@ -3562,14 +3609,14 @@
       <c r="E57" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>215</v>
+      <c r="F57" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>195</v>
+        <v>353</v>
       </c>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
@@ -3579,15 +3626,15 @@
       <c r="N57" s="14"/>
       <c r="O57" s="14"/>
     </row>
-    <row r="58" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" s="15" t="s">
-        <v>19</v>
+        <v>351</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>195</v>
+        <v>352</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>17</v>
@@ -3595,14 +3642,14 @@
       <c r="E58" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F58" s="14" t="s">
-        <v>215</v>
+      <c r="F58" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>195</v>
+        <v>353</v>
       </c>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
@@ -3617,25 +3664,25 @@
         <v>19</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>215</v>
+        <v>66</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
@@ -3645,30 +3692,30 @@
       <c r="N59" s="14"/>
       <c r="O59" s="14"/>
     </row>
-    <row r="60" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A60" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E60" s="15" t="s">
-        <v>159</v>
+      <c r="E60" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
@@ -3678,30 +3725,30 @@
       <c r="N60" s="14"/>
       <c r="O60" s="14"/>
     </row>
-    <row r="61" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A61" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>195</v>
+        <v>378</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>133</v>
+        <v>60</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>62</v>
+        <v>209</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
@@ -3716,24 +3763,26 @@
         <v>19</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>231</v>
+        <v>380</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>183</v>
+        <v>17</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="H62" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
       <c r="K62" s="14"/>
@@ -3747,24 +3796,26 @@
         <v>19</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>231</v>
+        <v>381</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>183</v>
+        <v>17</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="H63" s="14"/>
+        <v>213</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
       <c r="K63" s="14"/>
@@ -3773,15 +3824,15 @@
       <c r="N63" s="14"/>
       <c r="O63" s="14"/>
     </row>
-    <row r="64" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A64" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>195</v>
+        <v>382</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>17</v>
@@ -3789,14 +3840,14 @@
       <c r="E64" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F64" s="15" t="s">
-        <v>60</v>
+      <c r="F64" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>62</v>
+        <v>215</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
@@ -3808,25 +3859,28 @@
     </row>
     <row r="65" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A65" s="15" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>243</v>
+        <v>383</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>215</v>
+        <v>156</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>246</v>
+        <v>62</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>189</v>
       </c>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
@@ -3841,25 +3895,25 @@
         <v>19</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>195</v>
+        <v>384</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F66" s="14" t="s">
-        <v>215</v>
+        <v>156</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>245</v>
+        <v>62</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
@@ -3873,26 +3927,26 @@
       <c r="A67" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B67" s="15" t="s">
-        <v>248</v>
+      <c r="B67" s="16" t="s">
+        <v>385</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>195</v>
+        <v>387</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>60</v>
+        <v>178</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>250</v>
+        <v>389</v>
       </c>
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
@@ -3907,25 +3961,25 @@
         <v>19</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>251</v>
+        <v>386</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>195</v>
+        <v>388</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E68" s="15" t="s">
-        <v>132</v>
+      <c r="E68" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>253</v>
+        <v>390</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>195</v>
+        <v>389</v>
       </c>
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
@@ -3940,26 +3994,24 @@
         <v>19</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>252</v>
+        <v>392</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>195</v>
+        <v>391</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="H69" s="15" t="s">
-        <v>195</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H69" s="15"/>
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
       <c r="K69" s="14"/>
@@ -3968,30 +4020,27 @@
       <c r="N69" s="14"/>
       <c r="O69" s="14"/>
     </row>
-    <row r="70" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A70" s="15" t="s">
-        <v>19</v>
+        <v>225</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F70" s="15" t="s">
-        <v>183</v>
+        <v>17</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H70" s="15" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
       <c r="I70" s="14"/>
       <c r="J70" s="14"/>
@@ -4001,15 +4050,15 @@
       <c r="N70" s="14"/>
       <c r="O70" s="14"/>
     </row>
-    <row r="71" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A71" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>17</v>
@@ -4018,13 +4067,13 @@
         <v>60</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>62</v>
+        <v>233</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
@@ -4034,15 +4083,15 @@
       <c r="N71" s="14"/>
       <c r="O71" s="14"/>
     </row>
-    <row r="72" spans="1:15" ht="28" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A72" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>255</v>
+      <c r="B72" s="15" t="s">
+        <v>236</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>17</v>
@@ -4050,14 +4099,14 @@
       <c r="E72" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F72" s="14" t="s">
-        <v>215</v>
+      <c r="F72" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>62</v>
+        <v>237</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
@@ -4069,27 +4118,29 @@
     </row>
     <row r="73" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A73" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>264</v>
+        <v>189</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>265</v>
+        <v>130</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H73" s="14"/>
+        <v>241</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
       <c r="K73" s="14"/>
@@ -4100,27 +4151,29 @@
     </row>
     <row r="74" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A74" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>267</v>
+        <v>189</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>265</v>
+        <v>130</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H74" s="14"/>
+        <v>242</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I74" s="14"/>
       <c r="J74" s="14"/>
       <c r="K74" s="14"/>
@@ -4129,29 +4182,31 @@
       <c r="N74" s="14"/>
       <c r="O74" s="14"/>
     </row>
-    <row r="75" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A75" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>270</v>
+        <v>189</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>271</v>
+        <v>59</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>61</v>
+        <v>178</v>
       </c>
       <c r="G75" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H75" s="14"/>
+      <c r="H75" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I75" s="14"/>
       <c r="J75" s="14"/>
       <c r="K75" s="14"/>
@@ -4160,29 +4215,31 @@
       <c r="N75" s="14"/>
       <c r="O75" s="14"/>
     </row>
-    <row r="76" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A76" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>273</v>
+        <v>189</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="F76" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G76" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H76" s="14"/>
+      <c r="H76" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I76" s="14"/>
       <c r="J76" s="14"/>
       <c r="K76" s="14"/>
@@ -4191,47 +4248,54 @@
       <c r="N76" s="14"/>
       <c r="O76" s="14"/>
     </row>
-    <row r="77" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A77" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>276</v>
+        <v>189</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="F77" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="G77" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H77" s="14"/>
+      <c r="H77" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
-    </row>
-    <row r="78" spans="1:15" ht="56" x14ac:dyDescent="0.15">
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+    </row>
+    <row r="78" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A78" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>164</v>
+        <v>253</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>61</v>
@@ -4242,74 +4306,89 @@
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
-    </row>
-    <row r="79" spans="1:15" ht="84" x14ac:dyDescent="0.15">
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="14"/>
+    </row>
+    <row r="79" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A79" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="D79" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>159</v>
+        <v>253</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>281</v>
+        <v>62</v>
       </c>
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
-    </row>
-    <row r="80" spans="1:15" ht="84" x14ac:dyDescent="0.15">
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
+      <c r="N79" s="14"/>
+      <c r="O79" s="14"/>
+    </row>
+    <row r="80" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A80" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>161</v>
+        <v>256</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>159</v>
+        <v>259</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>283</v>
+        <v>62</v>
       </c>
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
-    </row>
-    <row r="81" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="14"/>
+    </row>
+    <row r="81" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A81" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>164</v>
+        <v>259</v>
       </c>
       <c r="F81" s="15" t="s">
         <v>61</v>
@@ -4320,22 +4399,27 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
-    </row>
-    <row r="82" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14"/>
+    </row>
+    <row r="82" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A82" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="D82" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F82" s="15" t="s">
         <v>61</v>
@@ -4347,21 +4431,21 @@
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
     </row>
-    <row r="83" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A83" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>288</v>
+        <v>160</v>
       </c>
       <c r="F83" s="15" t="s">
         <v>61</v>
@@ -4373,73 +4457,73 @@
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
     </row>
-    <row r="84" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:15" ht="84" x14ac:dyDescent="0.15">
       <c r="A84" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>288</v>
+        <v>156</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G84" s="15" t="s">
-        <v>62</v>
+        <v>269</v>
       </c>
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
     </row>
-    <row r="85" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:15" ht="84" x14ac:dyDescent="0.15">
       <c r="A85" s="15" t="s">
-        <v>293</v>
+        <v>23</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>294</v>
+        <v>158</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E85" s="14" t="s">
-        <v>74</v>
+      <c r="E85" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>62</v>
+        <v>271</v>
       </c>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
     </row>
-    <row r="86" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A86" s="15" t="s">
-        <v>293</v>
+        <v>23</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E86" s="14" t="s">
-        <v>74</v>
+      <c r="E86" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="F86" s="15" t="s">
         <v>61</v>
@@ -4451,21 +4535,21 @@
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
     </row>
-    <row r="87" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A87" s="15" t="s">
-        <v>293</v>
+        <v>23</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E87" s="14" t="s">
-        <v>74</v>
+      <c r="E87" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="F87" s="15" t="s">
         <v>61</v>
@@ -4477,21 +4561,21 @@
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
     </row>
-    <row r="88" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A88" s="15" t="s">
-        <v>293</v>
+        <v>23</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E88" s="14" t="s">
-        <v>74</v>
+      <c r="E88" s="15" t="s">
+        <v>276</v>
       </c>
       <c r="F88" s="15" t="s">
         <v>61</v>
@@ -4503,43 +4587,41 @@
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
     </row>
-    <row r="89" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A89" s="15" t="s">
-        <v>293</v>
+        <v>23</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E89" s="14" t="s">
-        <v>74</v>
+      <c r="E89" s="15" t="s">
+        <v>276</v>
       </c>
       <c r="F89" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G89" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="H89" s="15" t="s">
-        <v>304</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
     </row>
-    <row r="90" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A90" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>66</v>
@@ -4551,27 +4633,27 @@
         <v>61</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>281</v>
+        <v>62</v>
       </c>
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
     </row>
-    <row r="91" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A91" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E91" s="6" t="s">
-        <v>309</v>
+      <c r="E91" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F91" s="15" t="s">
         <v>61</v>
@@ -4583,21 +4665,21 @@
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
     </row>
-    <row r="92" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A92" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>309</v>
+      <c r="E92" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F92" s="15" t="s">
         <v>61</v>
@@ -4609,21 +4691,21 @@
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
     </row>
-    <row r="93" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A93" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E93" s="15" t="s">
-        <v>314</v>
+      <c r="E93" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F93" s="15" t="s">
         <v>61</v>
@@ -4635,73 +4717,75 @@
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
     </row>
-    <row r="94" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A94" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E94" s="15" t="s">
-        <v>314</v>
+      <c r="E94" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F94" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G94" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H94" s="14"/>
+        <v>354</v>
+      </c>
+      <c r="H94" s="15" t="s">
+        <v>292</v>
+      </c>
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
     </row>
-    <row r="95" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A95" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="B95" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="B95" s="16" t="s">
-        <v>317</v>
-      </c>
       <c r="C95" s="15" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E95" s="15" t="s">
-        <v>318</v>
+      <c r="E95" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="F95" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G95" s="15" t="s">
-        <v>62</v>
+        <v>269</v>
       </c>
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
     </row>
-    <row r="96" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A96" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E96" s="15" t="s">
-        <v>318</v>
+      <c r="E96" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="F96" s="15" t="s">
         <v>61</v>
@@ -4715,74 +4799,74 @@
     </row>
     <row r="97" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A97" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E97" s="15" t="s">
-        <v>324</v>
+      <c r="E97" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="F97" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G97" s="15" t="s">
-        <v>281</v>
+        <v>62</v>
       </c>
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
     </row>
-    <row r="98" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:10" ht="70" x14ac:dyDescent="0.15">
       <c r="A98" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E98" s="15" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="F98" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>359</v>
+        <v>62</v>
       </c>
       <c r="H98" s="14"/>
       <c r="I98" s="14"/>
       <c r="J98" s="14"/>
     </row>
-    <row r="99" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:10" ht="70" x14ac:dyDescent="0.15">
       <c r="A99" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E99" s="15" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>330</v>
+        <v>61</v>
       </c>
       <c r="G99" s="15" t="s">
         <v>62</v>
@@ -4791,24 +4875,24 @@
       <c r="I99" s="14"/>
       <c r="J99" s="14"/>
     </row>
-    <row r="100" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:10" ht="70" x14ac:dyDescent="0.15">
       <c r="A100" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E100" s="15" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="F100" s="15" t="s">
-        <v>330</v>
+        <v>61</v>
       </c>
       <c r="G100" s="15" t="s">
         <v>62</v>
@@ -4817,131 +4901,131 @@
       <c r="I100" s="14"/>
       <c r="J100" s="14"/>
     </row>
-    <row r="101" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:10" ht="70" x14ac:dyDescent="0.15">
       <c r="A101" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>336</v>
+        <v>66</v>
       </c>
       <c r="E101" s="15" t="s">
-        <v>60</v>
+        <v>306</v>
       </c>
       <c r="F101" s="15" t="s">
-        <v>335</v>
+        <v>61</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>334</v>
+        <v>62</v>
       </c>
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
     </row>
-    <row r="102" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A102" s="15" t="s">
-        <v>23</v>
+        <v>281</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>338</v>
+        <v>310</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>339</v>
+        <v>311</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E102" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F102" s="14" t="s">
-        <v>340</v>
+        <v>312</v>
+      </c>
+      <c r="F102" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>341</v>
+        <v>269</v>
       </c>
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
     </row>
-    <row r="103" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A103" s="15" t="s">
-        <v>23</v>
+        <v>281</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>342</v>
+        <v>313</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>343</v>
+        <v>314</v>
       </c>
       <c r="D103" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E103" s="15" t="s">
-        <v>159</v>
+        <v>312</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="G103" s="15" t="s">
-        <v>281</v>
+        <v>347</v>
       </c>
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
     </row>
-    <row r="104" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A104" s="15" t="s">
-        <v>23</v>
+        <v>281</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>344</v>
+        <v>315</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="D104" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E104" s="15" t="s">
-        <v>159</v>
+        <v>317</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>133</v>
+        <v>318</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>346</v>
+        <v>62</v>
       </c>
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="14"/>
     </row>
-    <row r="105" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A105" s="15" t="s">
-        <v>23</v>
+        <v>281</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>348</v>
+        <v>320</v>
       </c>
       <c r="D105" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E105" s="15" t="s">
-        <v>349</v>
+        <v>317</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>61</v>
+        <v>318</v>
       </c>
       <c r="G105" s="15" t="s">
-        <v>281</v>
+        <v>62</v>
       </c>
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
@@ -4949,39 +5033,39 @@
     </row>
     <row r="106" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A106" s="15" t="s">
-        <v>23</v>
+        <v>281</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>351</v>
+        <v>321</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>66</v>
+        <v>324</v>
       </c>
       <c r="E106" s="15" t="s">
-        <v>349</v>
+        <v>60</v>
       </c>
       <c r="F106" s="15" t="s">
-        <v>61</v>
+        <v>323</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>352</v>
+        <v>322</v>
       </c>
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="14"/>
     </row>
-    <row r="107" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A107" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="D107" s="15" t="s">
         <v>17</v>
@@ -4990,62 +5074,62 @@
         <v>60</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>215</v>
+        <v>328</v>
       </c>
       <c r="G107" s="15" t="s">
-        <v>62</v>
+        <v>329</v>
       </c>
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="14"/>
     </row>
-    <row r="108" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:10" ht="70" x14ac:dyDescent="0.15">
       <c r="A108" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E108" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F108" s="14" t="s">
-        <v>215</v>
+        <v>156</v>
+      </c>
+      <c r="F108" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="G108" s="15" t="s">
-        <v>62</v>
+        <v>269</v>
       </c>
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
       <c r="J108" s="14"/>
     </row>
-    <row r="109" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:10" ht="70" x14ac:dyDescent="0.15">
       <c r="A109" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>357</v>
+        <v>332</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="D109" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E109" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F109" s="14" t="s">
-        <v>215</v>
+        <v>156</v>
+      </c>
+      <c r="F109" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="G109" s="15" t="s">
-        <v>62</v>
+        <v>334</v>
       </c>
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
@@ -5056,83 +5140,159 @@
         <v>23</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>360</v>
+        <v>335</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E110" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F110" s="14" t="s">
-        <v>215</v>
+        <v>337</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G110" s="15" t="s">
-        <v>362</v>
+        <v>269</v>
       </c>
       <c r="H110" s="14"/>
       <c r="I110" s="14"/>
       <c r="J110" s="14"/>
     </row>
-    <row r="111" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A111" s="15"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
+    <row r="111" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="A111" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E111" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G111" s="15" t="s">
+        <v>340</v>
+      </c>
       <c r="H111" s="14"/>
       <c r="I111" s="14"/>
       <c r="J111" s="14"/>
     </row>
-    <row r="112" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A112" s="14"/>
-      <c r="B112" s="16"/>
-      <c r="C112" s="14"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
+    <row r="112" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+      <c r="A112" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F112" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G112" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
       <c r="J112" s="14"/>
     </row>
-    <row r="113" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A113" s="14"/>
-      <c r="B113" s="16"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
+    <row r="113" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+      <c r="A113" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E113" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F113" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G113" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="H113" s="14"/>
-    </row>
-    <row r="114" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A114" s="14"/>
-      <c r="B114" s="16"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
+      <c r="I113" s="14"/>
+      <c r="J113" s="14"/>
+    </row>
+    <row r="114" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+      <c r="A114" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G114" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="H114" s="14"/>
-    </row>
-    <row r="115" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A115" s="14"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="14"/>
+      <c r="I114" s="14"/>
+      <c r="J114" s="14"/>
+    </row>
+    <row r="115" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="A115" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E115" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F115" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G115" s="15" t="s">
+        <v>350</v>
+      </c>
       <c r="H115" s="14"/>
-    </row>
-    <row r="116" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A116" s="14"/>
+      <c r="I115" s="14"/>
+      <c r="J115" s="14"/>
+    </row>
+    <row r="116" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A116" s="15"/>
       <c r="B116" s="16"/>
       <c r="C116" s="14"/>
       <c r="D116" s="14"/>
@@ -5140,8 +5300,10 @@
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
       <c r="H116" s="14"/>
-    </row>
-    <row r="117" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I116" s="14"/>
+      <c r="J116" s="14"/>
+    </row>
+    <row r="117" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="14"/>
       <c r="B117" s="16"/>
       <c r="C117" s="14"/>
@@ -5150,8 +5312,10 @@
       <c r="F117" s="14"/>
       <c r="G117" s="14"/>
       <c r="H117" s="14"/>
-    </row>
-    <row r="118" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I117" s="14"/>
+      <c r="J117" s="14"/>
+    </row>
+    <row r="118" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="14"/>
       <c r="B118" s="16"/>
       <c r="C118" s="14"/>
@@ -5161,7 +5325,7 @@
       <c r="G118" s="14"/>
       <c r="H118" s="14"/>
     </row>
-    <row r="119" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="14"/>
       <c r="B119" s="16"/>
       <c r="C119" s="14"/>
@@ -5171,7 +5335,7 @@
       <c r="G119" s="14"/>
       <c r="H119" s="14"/>
     </row>
-    <row r="120" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="14"/>
       <c r="B120" s="16"/>
       <c r="C120" s="14"/>
@@ -5181,7 +5345,7 @@
       <c r="G120" s="14"/>
       <c r="H120" s="14"/>
     </row>
-    <row r="121" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="14"/>
       <c r="B121" s="16"/>
       <c r="C121" s="14"/>
@@ -5191,7 +5355,7 @@
       <c r="G121" s="14"/>
       <c r="H121" s="14"/>
     </row>
-    <row r="122" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="14"/>
       <c r="B122" s="16"/>
       <c r="C122" s="14"/>
@@ -5201,22 +5365,57 @@
       <c r="G122" s="14"/>
       <c r="H122" s="14"/>
     </row>
-    <row r="123" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B123" s="4"/>
-    </row>
-    <row r="124" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B124" s="4"/>
-    </row>
-    <row r="125" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B125" s="4"/>
-    </row>
-    <row r="126" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B126" s="4"/>
-    </row>
-    <row r="127" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B127" s="4"/>
-    </row>
-    <row r="128" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A123" s="14"/>
+      <c r="B123" s="16"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="14"/>
+    </row>
+    <row r="124" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A124" s="14"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="14"/>
+    </row>
+    <row r="125" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A125" s="14"/>
+      <c r="B125" s="16"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
+    </row>
+    <row r="126" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A126" s="14"/>
+      <c r="B126" s="16"/>
+      <c r="C126" s="14"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="14"/>
+    </row>
+    <row r="127" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A127" s="14"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="14"/>
+      <c r="G127" s="14"/>
+      <c r="H127" s="14"/>
+    </row>
+    <row r="128" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="B128" s="4"/>
     </row>
     <row r="129" spans="2:2" ht="13" x14ac:dyDescent="0.15">
@@ -7847,8 +8046,24 @@
     <row r="1004" spans="2:2" ht="13" x14ac:dyDescent="0.15">
       <c r="B1004" s="4"/>
     </row>
+    <row r="1005" spans="2:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1005" s="4"/>
+    </row>
+    <row r="1006" spans="2:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1006" s="4"/>
+    </row>
+    <row r="1007" spans="2:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1007" s="4"/>
+    </row>
+    <row r="1008" spans="2:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1008" s="4"/>
+    </row>
+    <row r="1009" spans="2:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1009" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7859,8 +8074,8 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7891,13 +8106,13 @@
         <v>77</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28" x14ac:dyDescent="0.15">
@@ -7989,7 +8204,7 @@
         <v>62</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.15">
@@ -8068,34 +8283,34 @@
         <v>19</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>235</v>
+        <v>393</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F11" s="15"/>
       <c r="H11" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>62</v>
@@ -8107,13 +8322,13 @@
         <v>18</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
add adhesive family qualities
</commit_message>
<xml_diff>
--- a/LOT_documents/FAIR Ontology Entities.xlsx
+++ b/LOT_documents/FAIR Ontology Entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ioannisdasoulas/Desktop/FAIR/Adhesive Selector/adhesive_ontology/LOT_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBF9CD4-1106-6B4B-97B1-31707B03EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D192F-E654-9E43-A7AC-8AA9A353CC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2600" yWindow="-17680" windowWidth="36480" windowHeight="17140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4120" yWindow="-18180" windowWidth="36480" windowHeight="17140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="414">
   <si>
     <t>Description</t>
   </si>
@@ -1228,6 +1228,66 @@
   </si>
   <si>
     <t>adhesion quality</t>
+  </si>
+  <si>
+    <t>ferroMetalAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with ferrous metals.</t>
+  </si>
+  <si>
+    <t>nonFerroMetalAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with non-ferrous metals.</t>
+  </si>
+  <si>
+    <t>steelAdhesionQuality</t>
+  </si>
+  <si>
+    <t>thermosetAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with thermoset.</t>
+  </si>
+  <si>
+    <t>thermoplasticAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with thermoplastic.</t>
+  </si>
+  <si>
+    <t>rubberAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with rubbers.</t>
+  </si>
+  <si>
+    <t>compositeAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with composites.</t>
+  </si>
+  <si>
+    <t>woodAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with wood.</t>
+  </si>
+  <si>
+    <t>glassAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with glass.</t>
+  </si>
+  <si>
+    <t>ceramicAdhesionQuality</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with ceramics.</t>
+  </si>
+  <si>
+    <t>A relation between an adhesive type and the quality of adhesion it achieves with steel.</t>
   </si>
 </sst>
 </file>
@@ -2006,7 +2066,7 @@
   </sheetPr>
   <dimension ref="A1:O1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="91" workbookViewId="0">
+    <sheetView topLeftCell="A99" zoomScale="91" workbookViewId="0">
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
@@ -8074,8 +8134,8 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8335,84 +8395,184 @@
       </c>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="14"/>
+    <row r="14" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14"/>
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="14"/>
+    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+      <c r="A16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14"/>
+    <row r="17" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="14"/>
+    <row r="18" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="14"/>
+    <row r="19" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="14"/>
+    <row r="20" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="14"/>
+    <row r="21" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="14"/>
+    <row r="22" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="14"/>
+    <row r="23" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -8561,5 +8721,6 @@
     <row r="58" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>